<commit_message>
updated preprocessing and main.py
</commit_message>
<xml_diff>
--- a/dicts/assets.xlsx
+++ b/dicts/assets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://goldenpearcapital.sharepoint.com/sites/GPResearchShareSite/Shared Documents/John/.Projects/.github/portfolio-dashboard/dicts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{7ACFF184-04AE-45FC-85B9-D64DE7D71570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A489512-16DD-42D6-BBBB-D4403CA5E829}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{7ACFF184-04AE-45FC-85B9-D64DE7D71570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAFDF9F3-4903-4E64-904C-224555C1494C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3FADFD0B-0116-4739-B48F-CA627278B549}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3FADFD0B-0116-4739-B48F-CA627278B549}"/>
   </bookViews>
   <sheets>
     <sheet name="assets" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <t>sector</t>
   </si>
   <si>
-    <t>asset_type</t>
-  </si>
-  <si>
     <t>coingecko_id</t>
   </si>
   <si>
@@ -473,6 +470,9 @@
   </si>
   <si>
     <t>JTO</t>
+  </si>
+  <si>
+    <t>bucket</t>
   </si>
 </sst>
 </file>
@@ -1335,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3A4D5B0-5786-4E71-9EA1-DD3E99C0DC0A}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,1390 +1355,1390 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
         <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
         <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
       <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
         <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" t="s">
-        <v>42</v>
-      </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
         <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
         <v>16</v>
       </c>
-      <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" t="s">
-        <v>17</v>
-      </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
         <v>7</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
         <v>16</v>
       </c>
-      <c r="C27" t="s">
-        <v>17</v>
-      </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
         <v>48</v>
-      </c>
-      <c r="B29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
         <v>50</v>
-      </c>
-      <c r="B30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
         <v>53</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" t="s">
         <v>54</v>
-      </c>
-      <c r="C32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" t="s">
         <v>57</v>
       </c>
-      <c r="B34" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" t="s">
-        <v>58</v>
-      </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" t="s">
         <v>59</v>
-      </c>
-      <c r="B35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" t="s">
-        <v>54</v>
-      </c>
-      <c r="E35" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" t="s">
         <v>61</v>
       </c>
-      <c r="B36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" t="s">
-        <v>62</v>
-      </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="s">
         <v>64</v>
-      </c>
-      <c r="B38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" t="s">
         <v>66</v>
-      </c>
-      <c r="B39" t="s">
-        <v>54</v>
-      </c>
-      <c r="C39" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" t="s">
-        <v>54</v>
-      </c>
-      <c r="E39" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" t="s">
         <v>69</v>
       </c>
-      <c r="B41" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" t="s">
-        <v>70</v>
-      </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
         <v>71</v>
-      </c>
-      <c r="B42" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" t="s">
-        <v>58</v>
-      </c>
-      <c r="D42" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" t="s">
         <v>16</v>
       </c>
-      <c r="C46" t="s">
-        <v>17</v>
-      </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
         <v>7</v>
-      </c>
-      <c r="D47" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" t="s">
+        <v>53</v>
+      </c>
+      <c r="E49" t="s">
         <v>79</v>
-      </c>
-      <c r="B49" t="s">
-        <v>79</v>
-      </c>
-      <c r="C49" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" t="s">
-        <v>54</v>
-      </c>
-      <c r="E49" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" t="s">
+        <v>57</v>
+      </c>
+      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" t="s">
         <v>81</v>
-      </c>
-      <c r="B50" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" t="s">
-        <v>58</v>
-      </c>
-      <c r="D50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D51" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" t="s">
         <v>6</v>
       </c>
-      <c r="B52" t="s">
-        <v>38</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>7</v>
       </c>
-      <c r="D52" t="s">
-        <v>8</v>
-      </c>
       <c r="E52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
         <v>85</v>
-      </c>
-      <c r="B53" t="s">
-        <v>38</v>
-      </c>
-      <c r="C53" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" t="s">
         <v>87</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>88</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" t="s">
         <v>89</v>
-      </c>
-      <c r="D54" t="s">
-        <v>89</v>
-      </c>
-      <c r="E54" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B55" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D55" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" t="s">
         <v>32</v>
-      </c>
-      <c r="C56" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" t="s">
         <v>93</v>
-      </c>
-      <c r="B57" t="s">
-        <v>93</v>
-      </c>
-      <c r="C57" t="s">
-        <v>70</v>
-      </c>
-      <c r="D57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" t="s">
         <v>16</v>
       </c>
-      <c r="C58" t="s">
-        <v>17</v>
-      </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" t="s">
+        <v>53</v>
+      </c>
+      <c r="E60" t="s">
         <v>97</v>
-      </c>
-      <c r="B60" t="s">
-        <v>54</v>
-      </c>
-      <c r="C60" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" t="s">
-        <v>54</v>
-      </c>
-      <c r="E60" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" t="s">
         <v>16</v>
       </c>
-      <c r="C61" t="s">
-        <v>17</v>
-      </c>
       <c r="D61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" t="s">
         <v>100</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>101</v>
       </c>
-      <c r="C62" t="s">
-        <v>102</v>
-      </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" t="s">
+        <v>69</v>
+      </c>
+      <c r="D64" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" t="s">
         <v>104</v>
-      </c>
-      <c r="B64" t="s">
-        <v>104</v>
-      </c>
-      <c r="C64" t="s">
-        <v>70</v>
-      </c>
-      <c r="D64" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" t="s">
         <v>7</v>
       </c>
-      <c r="D65" t="s">
-        <v>8</v>
-      </c>
       <c r="E65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" t="s">
+        <v>37</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" t="s">
         <v>106</v>
-      </c>
-      <c r="B66" t="s">
-        <v>38</v>
-      </c>
-      <c r="C66" t="s">
-        <v>7</v>
-      </c>
-      <c r="D66" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B67" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" t="s">
         <v>16</v>
       </c>
-      <c r="C67" t="s">
-        <v>17</v>
-      </c>
       <c r="D67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B68" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>109</v>
+      </c>
+      <c r="B69" t="s">
+        <v>109</v>
+      </c>
+      <c r="C69" t="s">
+        <v>69</v>
+      </c>
+      <c r="D69" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" t="s">
         <v>110</v>
-      </c>
-      <c r="B69" t="s">
-        <v>110</v>
-      </c>
-      <c r="C69" t="s">
-        <v>70</v>
-      </c>
-      <c r="D69" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" t="s">
         <v>16</v>
       </c>
-      <c r="C70" t="s">
-        <v>17</v>
-      </c>
       <c r="D70" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" t="s">
+        <v>16</v>
+      </c>
+      <c r="D71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E71" t="s">
         <v>113</v>
-      </c>
-      <c r="B71" t="s">
-        <v>16</v>
-      </c>
-      <c r="C71" t="s">
-        <v>17</v>
-      </c>
-      <c r="D71" t="s">
-        <v>16</v>
-      </c>
-      <c r="E71" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" t="s">
         <v>16</v>
       </c>
-      <c r="C72" t="s">
-        <v>17</v>
-      </c>
       <c r="D72" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E72" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>115</v>
+      </c>
+      <c r="B73" t="s">
+        <v>115</v>
+      </c>
+      <c r="C73" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" t="s">
         <v>116</v>
-      </c>
-      <c r="B73" t="s">
-        <v>116</v>
-      </c>
-      <c r="C73" t="s">
-        <v>62</v>
-      </c>
-      <c r="D73" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C74" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" t="s">
+        <v>118</v>
+      </c>
+      <c r="C75" t="s">
+        <v>61</v>
+      </c>
+      <c r="D75" t="s">
+        <v>10</v>
+      </c>
+      <c r="E75" t="s">
         <v>119</v>
-      </c>
-      <c r="B75" t="s">
-        <v>119</v>
-      </c>
-      <c r="C75" t="s">
-        <v>62</v>
-      </c>
-      <c r="D75" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>120</v>
+      </c>
+      <c r="B76" t="s">
+        <v>120</v>
+      </c>
+      <c r="C76" t="s">
+        <v>69</v>
+      </c>
+      <c r="D76" t="s">
+        <v>10</v>
+      </c>
+      <c r="E76" t="s">
         <v>121</v>
-      </c>
-      <c r="B76" t="s">
-        <v>121</v>
-      </c>
-      <c r="C76" t="s">
-        <v>70</v>
-      </c>
-      <c r="D76" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" t="s">
+        <v>122</v>
+      </c>
+      <c r="C77" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" t="s">
         <v>123</v>
-      </c>
-      <c r="B77" t="s">
-        <v>123</v>
-      </c>
-      <c r="C77" t="s">
-        <v>14</v>
-      </c>
-      <c r="D77" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B78" t="s">
+        <v>15</v>
+      </c>
+      <c r="C78" t="s">
         <v>16</v>
       </c>
-      <c r="C78" t="s">
-        <v>17</v>
-      </c>
       <c r="D78" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" t="s">
+        <v>125</v>
+      </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" t="s">
+        <v>10</v>
+      </c>
+      <c r="E79" t="s">
         <v>126</v>
-      </c>
-      <c r="B79" t="s">
-        <v>126</v>
-      </c>
-      <c r="C79" t="s">
-        <v>10</v>
-      </c>
-      <c r="D79" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>127</v>
+      </c>
+      <c r="B80" t="s">
+        <v>53</v>
+      </c>
+      <c r="C80" t="s">
+        <v>16</v>
+      </c>
+      <c r="D80" t="s">
+        <v>53</v>
+      </c>
+      <c r="E80" t="s">
         <v>128</v>
-      </c>
-      <c r="B80" t="s">
-        <v>54</v>
-      </c>
-      <c r="C80" t="s">
-        <v>17</v>
-      </c>
-      <c r="D80" t="s">
-        <v>54</v>
-      </c>
-      <c r="E80" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" t="s">
+        <v>129</v>
+      </c>
+      <c r="C81" t="s">
+        <v>69</v>
+      </c>
+      <c r="D81" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" t="s">
         <v>130</v>
-      </c>
-      <c r="B81" t="s">
-        <v>130</v>
-      </c>
-      <c r="C81" t="s">
-        <v>70</v>
-      </c>
-      <c r="D81" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" t="s">
+        <v>131</v>
+      </c>
+      <c r="C82" t="s">
         <v>132</v>
       </c>
-      <c r="B82" t="s">
-        <v>132</v>
-      </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" t="s">
         <v>133</v>
-      </c>
-      <c r="D82" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>134</v>
+      </c>
+      <c r="B83" t="s">
+        <v>134</v>
+      </c>
+      <c r="C83" t="s">
+        <v>69</v>
+      </c>
+      <c r="D83" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" t="s">
         <v>135</v>
-      </c>
-      <c r="B83" t="s">
-        <v>135</v>
-      </c>
-      <c r="C83" t="s">
-        <v>70</v>
-      </c>
-      <c r="D83" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>136</v>
+      </c>
+      <c r="B84" t="s">
+        <v>136</v>
+      </c>
+      <c r="C84" t="s">
+        <v>61</v>
+      </c>
+      <c r="D84" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" t="s">
         <v>137</v>
-      </c>
-      <c r="B84" t="s">
-        <v>137</v>
-      </c>
-      <c r="C84" t="s">
-        <v>62</v>
-      </c>
-      <c r="D84" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B85" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C85" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D85" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>139</v>
+      </c>
+      <c r="B86" t="s">
+        <v>139</v>
+      </c>
+      <c r="C86" t="s">
         <v>140</v>
       </c>
-      <c r="B86" t="s">
-        <v>140</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" t="s">
         <v>141</v>
-      </c>
-      <c r="D86" t="s">
-        <v>11</v>
-      </c>
-      <c r="E86" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>142</v>
+      </c>
+      <c r="B87" t="s">
+        <v>142</v>
+      </c>
+      <c r="D87" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" t="s">
         <v>143</v>
-      </c>
-      <c r="B87" t="s">
-        <v>143</v>
-      </c>
-      <c r="D87" t="s">
-        <v>11</v>
-      </c>
-      <c r="E87" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>144</v>
+      </c>
+      <c r="B88" t="s">
+        <v>144</v>
+      </c>
+      <c r="C88" t="s">
+        <v>69</v>
+      </c>
+      <c r="D88" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" t="s">
         <v>145</v>
-      </c>
-      <c r="B88" t="s">
-        <v>145</v>
-      </c>
-      <c r="C88" t="s">
-        <v>70</v>
-      </c>
-      <c r="D88" t="s">
-        <v>11</v>
-      </c>
-      <c r="E88" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B89" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" t="s">
         <v>16</v>
       </c>
-      <c r="C89" t="s">
-        <v>17</v>
-      </c>
       <c r="D89" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B90" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" t="s">
         <v>16</v>
       </c>
-      <c r="C90" t="s">
-        <v>17</v>
-      </c>
       <c r="D90" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B91" t="s">
+        <v>15</v>
+      </c>
+      <c r="C91" t="s">
         <v>16</v>
       </c>
-      <c r="C91" t="s">
-        <v>17</v>
-      </c>
       <c r="D91" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2747,15 +2747,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009CA2208F381845469048B4BD48A230FB" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8d41f01092630eeb17f7f45639ef6ba2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac1e3db1-1ad1-477c-a04d-2064aa9a5979" xmlns:ns3="74c9d6e8-536c-419c-a338-2519a9e68930" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64bd5bbfef86a54cc7f921d64a1f416e" ns2:_="" ns3:_="">
     <xsd:import namespace="ac1e3db1-1ad1-477c-a04d-2064aa9a5979"/>
@@ -2984,7 +2975,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="ac1e3db1-1ad1-477c-a04d-2064aa9a5979">
@@ -2995,15 +2986,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79E67843-A277-4CB1-8C1D-C824DA2F2CB0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1FBE437-42DA-49CD-A8F8-81BADCBDF61F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3022,7 +3014,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B35602E-4B38-480F-A6A8-5F371E3D10EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3031,4 +3023,12 @@
     <ds:schemaRef ds:uri="74c9d6e8-536c-419c-a338-2519a9e68930"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79E67843-A277-4CB1-8C1D-C824DA2F2CB0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated apis, asset dictionary, and added cost_basis and amount_change columns
</commit_message>
<xml_diff>
--- a/dicts/assets.xlsx
+++ b/dicts/assets.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://goldenpearcapital.sharepoint.com/sites/GPResearchShareSite/Shared Documents/John/.Projects/.github/portfolio-dashboard/dicts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{7ACFF184-04AE-45FC-85B9-D64DE7D71570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAFDF9F3-4903-4E64-904C-224555C1494C}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{7ACFF184-04AE-45FC-85B9-D64DE7D71570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B94314E5-9207-40F6-AF77-A1355DB5D2AE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3FADFD0B-0116-4739-B48F-CA627278B549}"/>
   </bookViews>
   <sheets>
     <sheet name="assets" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="202">
   <si>
     <t>symbol</t>
   </si>
@@ -473,6 +486,159 @@
   </si>
   <si>
     <t>bucket</t>
+  </si>
+  <si>
+    <t>stkLYRA</t>
+  </si>
+  <si>
+    <t>esGMX</t>
+  </si>
+  <si>
+    <t>PED</t>
+  </si>
+  <si>
+    <t>FXTL</t>
+  </si>
+  <si>
+    <t>MIM</t>
+  </si>
+  <si>
+    <t>EIGEN</t>
+  </si>
+  <si>
+    <t>SMOG</t>
+  </si>
+  <si>
+    <t>PREMIA</t>
+  </si>
+  <si>
+    <t>vBSWAP</t>
+  </si>
+  <si>
+    <t>TED</t>
+  </si>
+  <si>
+    <t>PLS</t>
+  </si>
+  <si>
+    <t>DrumCat</t>
+  </si>
+  <si>
+    <t>9MM</t>
+  </si>
+  <si>
+    <t>BEW</t>
+  </si>
+  <si>
+    <t>PONP</t>
+  </si>
+  <si>
+    <t>SHB</t>
+  </si>
+  <si>
+    <t>BLOOM</t>
+  </si>
+  <si>
+    <t>OHNO</t>
+  </si>
+  <si>
+    <t>FaceDAO</t>
+  </si>
+  <si>
+    <t>MOTHER</t>
+  </si>
+  <si>
+    <t>DAWAE</t>
+  </si>
+  <si>
+    <t>WAZ</t>
+  </si>
+  <si>
+    <t>PCAT</t>
+  </si>
+  <si>
+    <t>GROYPER</t>
+  </si>
+  <si>
+    <t>TKX</t>
+  </si>
+  <si>
+    <t>PIG</t>
+  </si>
+  <si>
+    <t>NDQ</t>
+  </si>
+  <si>
+    <t>SHEESHA</t>
+  </si>
+  <si>
+    <t>OOMER</t>
+  </si>
+  <si>
+    <t>WGC</t>
+  </si>
+  <si>
+    <t>SONNE</t>
+  </si>
+  <si>
+    <t>BUSD</t>
+  </si>
+  <si>
+    <t>AVAX</t>
+  </si>
+  <si>
+    <t>PBRO</t>
+  </si>
+  <si>
+    <t>OX</t>
+  </si>
+  <si>
+    <t>BASED</t>
+  </si>
+  <si>
+    <t>BENTO</t>
+  </si>
+  <si>
+    <t>GAST</t>
+  </si>
+  <si>
+    <t>PUMP</t>
+  </si>
+  <si>
+    <t>LOA</t>
+  </si>
+  <si>
+    <t>WMATIC</t>
+  </si>
+  <si>
+    <t>UNCLE</t>
+  </si>
+  <si>
+    <t>HOPPY</t>
+  </si>
+  <si>
+    <t>TrumpCash</t>
+  </si>
+  <si>
+    <t>MNT</t>
+  </si>
+  <si>
+    <t>XVS</t>
+  </si>
+  <si>
+    <t>CNC</t>
+  </si>
+  <si>
+    <t>USDC.e</t>
+  </si>
+  <si>
+    <t>GMX</t>
+  </si>
+  <si>
+    <t>BSWAP</t>
+  </si>
+  <si>
+    <t>DeFi - Yield Aggregator</t>
   </si>
 </sst>
 </file>
@@ -1333,15 +1499,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3A4D5B0-5786-4E71-9EA1-DD3E99C0DC0A}">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2675,6 +2842,9 @@
       <c r="B87" t="s">
         <v>142</v>
       </c>
+      <c r="C87" t="s">
+        <v>24</v>
+      </c>
       <c r="D87" t="s">
         <v>10</v>
       </c>
@@ -2739,6 +2909,676 @@
       </c>
       <c r="D91" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>151</v>
+      </c>
+      <c r="B92" t="s">
+        <v>60</v>
+      </c>
+      <c r="C92" t="s">
+        <v>201</v>
+      </c>
+      <c r="D92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>152</v>
+      </c>
+      <c r="B93" t="s">
+        <v>199</v>
+      </c>
+      <c r="C93" t="s">
+        <v>61</v>
+      </c>
+      <c r="D93" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>153</v>
+      </c>
+      <c r="B94" t="s">
+        <v>153</v>
+      </c>
+      <c r="C94" t="s">
+        <v>69</v>
+      </c>
+      <c r="D94" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>154</v>
+      </c>
+      <c r="B95" t="s">
+        <v>154</v>
+      </c>
+      <c r="C95" t="s">
+        <v>13</v>
+      </c>
+      <c r="D95" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>155</v>
+      </c>
+      <c r="B96" t="s">
+        <v>37</v>
+      </c>
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>156</v>
+      </c>
+      <c r="B97" t="s">
+        <v>156</v>
+      </c>
+      <c r="C97" t="s">
+        <v>13</v>
+      </c>
+      <c r="D97" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>157</v>
+      </c>
+      <c r="B98" t="s">
+        <v>157</v>
+      </c>
+      <c r="C98" t="s">
+        <v>69</v>
+      </c>
+      <c r="D98" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>158</v>
+      </c>
+      <c r="B99" t="s">
+        <v>158</v>
+      </c>
+      <c r="C99" t="s">
+        <v>61</v>
+      </c>
+      <c r="D99" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>159</v>
+      </c>
+      <c r="B100" t="s">
+        <v>200</v>
+      </c>
+      <c r="C100" t="s">
+        <v>24</v>
+      </c>
+      <c r="D100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>160</v>
+      </c>
+      <c r="B101" t="s">
+        <v>160</v>
+      </c>
+      <c r="C101" t="s">
+        <v>69</v>
+      </c>
+      <c r="D101" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>161</v>
+      </c>
+      <c r="B102" t="s">
+        <v>161</v>
+      </c>
+      <c r="C102" t="s">
+        <v>16</v>
+      </c>
+      <c r="D102" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>162</v>
+      </c>
+      <c r="B103" t="str">
+        <f>A103</f>
+        <v>DrumCat</v>
+      </c>
+      <c r="C103" t="s">
+        <v>69</v>
+      </c>
+      <c r="D103" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>163</v>
+      </c>
+      <c r="B104" t="str">
+        <f t="shared" ref="B104:B138" si="0">A104</f>
+        <v>9MM</v>
+      </c>
+      <c r="C104" t="s">
+        <v>69</v>
+      </c>
+      <c r="D104" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>164</v>
+      </c>
+      <c r="B105" t="str">
+        <f t="shared" si="0"/>
+        <v>BEW</v>
+      </c>
+      <c r="C105" t="s">
+        <v>69</v>
+      </c>
+      <c r="D105" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>165</v>
+      </c>
+      <c r="B106" t="str">
+        <f t="shared" si="0"/>
+        <v>PONP</v>
+      </c>
+      <c r="D106" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>166</v>
+      </c>
+      <c r="B107" t="str">
+        <f t="shared" si="0"/>
+        <v>SHB</v>
+      </c>
+      <c r="D107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>167</v>
+      </c>
+      <c r="B108" t="str">
+        <f t="shared" si="0"/>
+        <v>BLOOM</v>
+      </c>
+      <c r="D108" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>168</v>
+      </c>
+      <c r="B109" t="str">
+        <f t="shared" si="0"/>
+        <v>OHNO</v>
+      </c>
+      <c r="D109" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>169</v>
+      </c>
+      <c r="B110" t="str">
+        <f t="shared" si="0"/>
+        <v>FaceDAO</v>
+      </c>
+      <c r="D110" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>170</v>
+      </c>
+      <c r="B111" t="str">
+        <f t="shared" si="0"/>
+        <v>MOTHER</v>
+      </c>
+      <c r="C111" t="s">
+        <v>69</v>
+      </c>
+      <c r="D111" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>171</v>
+      </c>
+      <c r="B112" t="str">
+        <f t="shared" si="0"/>
+        <v>DAWAE</v>
+      </c>
+      <c r="D112" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>172</v>
+      </c>
+      <c r="B113" t="str">
+        <f t="shared" si="0"/>
+        <v>WAZ</v>
+      </c>
+      <c r="D113" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>173</v>
+      </c>
+      <c r="B114" t="str">
+        <f t="shared" si="0"/>
+        <v>PCAT</v>
+      </c>
+      <c r="C114" t="s">
+        <v>69</v>
+      </c>
+      <c r="D114" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>174</v>
+      </c>
+      <c r="B115" t="str">
+        <f t="shared" si="0"/>
+        <v>GROYPER</v>
+      </c>
+      <c r="C115" t="s">
+        <v>69</v>
+      </c>
+      <c r="D115" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>175</v>
+      </c>
+      <c r="B116" t="str">
+        <f t="shared" si="0"/>
+        <v>TKX</v>
+      </c>
+      <c r="D116" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>176</v>
+      </c>
+      <c r="B117" t="str">
+        <f t="shared" si="0"/>
+        <v>PIG</v>
+      </c>
+      <c r="D117" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>177</v>
+      </c>
+      <c r="B118" t="str">
+        <f t="shared" si="0"/>
+        <v>NDQ</v>
+      </c>
+      <c r="D118" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>178</v>
+      </c>
+      <c r="B119" t="str">
+        <f t="shared" si="0"/>
+        <v>SHEESHA</v>
+      </c>
+      <c r="C119" t="s">
+        <v>140</v>
+      </c>
+      <c r="D119" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>179</v>
+      </c>
+      <c r="B120" t="str">
+        <f t="shared" si="0"/>
+        <v>OOMER</v>
+      </c>
+      <c r="C120" t="s">
+        <v>69</v>
+      </c>
+      <c r="D120" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>180</v>
+      </c>
+      <c r="B121" t="str">
+        <f t="shared" si="0"/>
+        <v>WGC</v>
+      </c>
+      <c r="D121" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>181</v>
+      </c>
+      <c r="B122" t="str">
+        <f t="shared" si="0"/>
+        <v>SONNE</v>
+      </c>
+      <c r="C122" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>182</v>
+      </c>
+      <c r="B123" t="s">
+        <v>37</v>
+      </c>
+      <c r="C123" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>183</v>
+      </c>
+      <c r="B124" t="str">
+        <f t="shared" si="0"/>
+        <v>AVAX</v>
+      </c>
+      <c r="C124" t="s">
+        <v>16</v>
+      </c>
+      <c r="D124" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>184</v>
+      </c>
+      <c r="B125" t="str">
+        <f t="shared" si="0"/>
+        <v>PBRO</v>
+      </c>
+      <c r="C125" t="s">
+        <v>69</v>
+      </c>
+      <c r="D125" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>185</v>
+      </c>
+      <c r="B126" t="str">
+        <f t="shared" si="0"/>
+        <v>OX</v>
+      </c>
+      <c r="C126" t="s">
+        <v>61</v>
+      </c>
+      <c r="D126" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>186</v>
+      </c>
+      <c r="B127" t="str">
+        <f t="shared" si="0"/>
+        <v>BASED</v>
+      </c>
+      <c r="C127" t="s">
+        <v>69</v>
+      </c>
+      <c r="D127" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>187</v>
+      </c>
+      <c r="B128" t="str">
+        <f t="shared" si="0"/>
+        <v>BENTO</v>
+      </c>
+      <c r="C128" t="s">
+        <v>69</v>
+      </c>
+      <c r="D128" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>188</v>
+      </c>
+      <c r="B129" t="str">
+        <f t="shared" si="0"/>
+        <v>GAST</v>
+      </c>
+      <c r="C129" t="s">
+        <v>69</v>
+      </c>
+      <c r="D129" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>189</v>
+      </c>
+      <c r="B130" t="str">
+        <f t="shared" si="0"/>
+        <v>PUMP</v>
+      </c>
+      <c r="C130" t="s">
+        <v>69</v>
+      </c>
+      <c r="D130" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>190</v>
+      </c>
+      <c r="B131" t="str">
+        <f t="shared" si="0"/>
+        <v>LOA</v>
+      </c>
+      <c r="C131" t="s">
+        <v>69</v>
+      </c>
+      <c r="D131" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>191</v>
+      </c>
+      <c r="B132" t="s">
+        <v>62</v>
+      </c>
+      <c r="C132" t="s">
+        <v>13</v>
+      </c>
+      <c r="D132" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>192</v>
+      </c>
+      <c r="B133" t="str">
+        <f t="shared" si="0"/>
+        <v>UNCLE</v>
+      </c>
+      <c r="C133" t="s">
+        <v>69</v>
+      </c>
+      <c r="D133" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>193</v>
+      </c>
+      <c r="B134" t="str">
+        <f t="shared" si="0"/>
+        <v>HOPPY</v>
+      </c>
+      <c r="C134" t="s">
+        <v>69</v>
+      </c>
+      <c r="D134" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>194</v>
+      </c>
+      <c r="B135" t="str">
+        <f t="shared" si="0"/>
+        <v>TrumpCash</v>
+      </c>
+      <c r="C135" t="s">
+        <v>69</v>
+      </c>
+      <c r="D135" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>195</v>
+      </c>
+      <c r="B136" t="str">
+        <f t="shared" si="0"/>
+        <v>MNT</v>
+      </c>
+      <c r="D136" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>196</v>
+      </c>
+      <c r="B137" t="str">
+        <f t="shared" si="0"/>
+        <v>XVS</v>
+      </c>
+      <c r="C137" t="s">
+        <v>9</v>
+      </c>
+      <c r="D137" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>197</v>
+      </c>
+      <c r="B138" t="str">
+        <f t="shared" si="0"/>
+        <v>CNC</v>
+      </c>
+      <c r="C138" t="s">
+        <v>201</v>
+      </c>
+      <c r="D138" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>198</v>
+      </c>
+      <c r="B139" t="s">
+        <v>37</v>
+      </c>
+      <c r="C139" t="s">
+        <v>6</v>
+      </c>
+      <c r="D139" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2747,6 +3587,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ac1e3db1-1ad1-477c-a04d-2064aa9a5979">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="74c9d6e8-536c-419c-a338-2519a9e68930" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009CA2208F381845469048B4BD48A230FB" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8d41f01092630eeb17f7f45639ef6ba2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ac1e3db1-1ad1-477c-a04d-2064aa9a5979" xmlns:ns3="74c9d6e8-536c-419c-a338-2519a9e68930" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64bd5bbfef86a54cc7f921d64a1f416e" ns2:_="" ns3:_="">
     <xsd:import namespace="ac1e3db1-1ad1-477c-a04d-2064aa9a5979"/>
@@ -2975,17 +3826,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ac1e3db1-1ad1-477c-a04d-2064aa9a5979">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="74c9d6e8-536c-419c-a338-2519a9e68930" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2996,6 +3836,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B35602E-4B38-480F-A6A8-5F371E3D10EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ac1e3db1-1ad1-477c-a04d-2064aa9a5979"/>
+    <ds:schemaRef ds:uri="74c9d6e8-536c-419c-a338-2519a9e68930"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1FBE437-42DA-49CD-A8F8-81BADCBDF61F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3014,17 +3865,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B35602E-4B38-480F-A6A8-5F371E3D10EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ac1e3db1-1ad1-477c-a04d-2064aa9a5979"/>
-    <ds:schemaRef ds:uri="74c9d6e8-536c-419c-a338-2519a9e68930"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79E67843-A277-4CB1-8C1D-C824DA2F2CB0}">
   <ds:schemaRefs>

</xml_diff>